<commit_message>
journal de travail update
</commit_message>
<xml_diff>
--- a/doc/journal de travail MA-20.xlsx
+++ b/doc/journal de travail MA-20.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Aide de la part de Sebastien pour améliorer visuellement le tableau graphique</t>
+  </si>
+  <si>
+    <t>Affichage des bateaux coulés et messages de victoire, le nombre de cases ratés quand tous les bateaux sont coulés</t>
   </si>
 </sst>
 </file>
@@ -539,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,16 +829,26 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>43902</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="4">
+        <v>43903</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>

</xml_diff>

<commit_message>
Création de conditions si le chiffre est supérieur à 10 (WIP)
</commit_message>
<xml_diff>
--- a/doc/journal de travail MA-20.xlsx
+++ b/doc/journal de travail MA-20.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>Affichage des bateaux coulés et messages de victoire, le nombre de cases ratés quand tous les bateaux sont coulés</t>
+  </si>
+  <si>
+    <t>J'ai rajouté le nombre de vies totaux des bateaux après une inspiration de Sebastien Moraz. (Parce que c'est quand même pratique de voir les points de vie)</t>
+  </si>
+  <si>
+    <t>Création des conditions si le chiffre choisi est inférieur à 10 et affichage des points de vie des bateaux</t>
+  </si>
+  <si>
+    <t>j'ai essayé de mettre des couleurs aux tâches touchées.</t>
+  </si>
+  <si>
+    <t>Toujours entrain d'essayer de mettre une couleur aux cases touchées</t>
   </si>
 </sst>
 </file>
@@ -543,7 +555,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +841,7 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>43902</v>
       </c>
@@ -842,18 +854,30 @@
       <c r="D16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43903</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="1"/>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>

</xml_diff>

<commit_message>
Corrections de bugs divers
</commit_message>
<xml_diff>
--- a/doc/journal de travail MA-20.xlsx
+++ b/doc/journal de travail MA-20.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MA-20\BatailleNavale\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPNV\MA-20\Bataille-Navale\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C2BBE8-ABAD-404A-9CB2-069232E73EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17295" windowHeight="11520"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -147,12 +148,21 @@
   </si>
   <si>
     <t>Toujours entrain d'essayer de mettre une couleur aux cases touchées</t>
+  </si>
+  <si>
+    <t>Corrections de bugs</t>
+  </si>
+  <si>
+    <t>30mins</t>
+  </si>
+  <si>
+    <t>Quand on retire sur une case un message affiche qu'on a déjà tiré dessus. Une redirection sur le menu a aussi été ajoutée.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,26 +561,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="46.88671875" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -590,7 +600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>43887</v>
       </c>
@@ -611,7 +621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>43887</v>
       </c>
@@ -629,7 +639,7 @@
       </c>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43888</v>
       </c>
@@ -647,7 +657,7 @@
       </c>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43888</v>
       </c>
@@ -665,7 +675,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43889</v>
       </c>
@@ -683,7 +693,7 @@
       </c>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43894</v>
       </c>
@@ -701,7 +711,7 @@
       </c>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43894</v>
       </c>
@@ -719,7 +729,7 @@
       </c>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>43894</v>
       </c>
@@ -737,7 +747,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>43895</v>
       </c>
@@ -755,7 +765,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>43896</v>
       </c>
@@ -773,7 +783,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>43901</v>
       </c>
@@ -791,7 +801,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43901</v>
       </c>
@@ -807,7 +817,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>43901</v>
       </c>
@@ -823,7 +833,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43901</v>
       </c>
@@ -841,7 +851,7 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43902</v>
       </c>
@@ -859,7 +869,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43903</v>
       </c>
@@ -879,15 +889,25 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="5"/>
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>43905</v>
+      </c>
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -895,7 +915,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -903,7 +923,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -911,7 +931,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -919,7 +939,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -927,7 +947,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>

</xml_diff>

<commit_message>
Autres corrections de bugs, addition d'une couleur et revue des commentaires
</commit_message>
<xml_diff>
--- a/doc/journal de travail MA-20.xlsx
+++ b/doc/journal de travail MA-20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPNV\MA-20\Bataille-Navale\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C2BBE8-ABAD-404A-9CB2-069232E73EB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F992E5D-115A-4406-8D9F-8C96DFCB7516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -157,13 +157,31 @@
   </si>
   <si>
     <t>Quand on retire sur une case un message affiche qu'on a déjà tiré dessus. Une redirection sur le menu a aussi été ajoutée.</t>
+  </si>
+  <si>
+    <t>Finalisation des corrections de bugs</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Finalisation des bugs, quand on choisis un chiffre supérieur à 10, il redemande jusqu'à ce que le chiffre soit inférieur de 10 est fonctionnel. Quelques test avec les couleurs ont été faites.      J'ai trouvé comment mettre de la couleur sur cette source :  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://stackoverflow.com/questions/2841539/there-was-a-function-in-c-to-adjust-background-color-it-was-actually-a-dos-com</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +192,13 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -564,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,68 +877,78 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="A16" s="12">
         <v>43902</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="13">
         <v>5</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+      <c r="A17" s="12">
         <v>43903</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="13">
         <v>5</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="A18" s="12">
         <v>43905</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="13">
         <v>5</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="1"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="12">
+        <v>43906</v>
+      </c>
+      <c r="B19" s="13">
+        <v>6</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>

</xml_diff>

<commit_message>
Création de nom d'utilisateur sans fichier
</commit_message>
<xml_diff>
--- a/doc/journal de travail MA-20.xlsx
+++ b/doc/journal de travail MA-20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPNV\MA-20\Bataille-Navale\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marina\Documents\CPNV\MA-20\Bataille-Navale\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1487A47D-81EC-41BC-AFD9-5F3696A12984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B854AD58-BBBA-453D-ACEE-CBAD09464BF0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="3348" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -175,6 +175,15 @@
       </rPr>
       <t>https://stackoverflow.com/questions/2841539/there-was-a-function-in-c-to-adjust-background-color-it-was-actually-a-dos-com</t>
     </r>
+  </si>
+  <si>
+    <t>2h15</t>
+  </si>
+  <si>
+    <t>Visualition de vidéos pour comment créer des fichiers dans le jeu, et création d'utilisateur avant le début de la partie</t>
+  </si>
+  <si>
+    <t>J'ai visualisé des vidéos pour comment faire des fichiers et comment y écrire à l'intérieur, et le programme demande si l'utilisateur veut entrer un nom ou pas et l'affiche pendant le jeu et la fin du jeu dans le message de victoire</t>
   </si>
 </sst>
 </file>
@@ -590,22 +599,22 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B19" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="48.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="46.88671875" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -625,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>43887</v>
       </c>
@@ -646,7 +655,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>43887</v>
       </c>
@@ -664,7 +673,7 @@
       </c>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43888</v>
       </c>
@@ -682,7 +691,7 @@
       </c>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43888</v>
       </c>
@@ -700,7 +709,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43889</v>
       </c>
@@ -718,7 +727,7 @@
       </c>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43894</v>
       </c>
@@ -736,7 +745,7 @@
       </c>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43894</v>
       </c>
@@ -754,7 +763,7 @@
       </c>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>43894</v>
       </c>
@@ -772,7 +781,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>43895</v>
       </c>
@@ -790,7 +799,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>43896</v>
       </c>
@@ -808,7 +817,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>43901</v>
       </c>
@@ -826,7 +835,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43901</v>
       </c>
@@ -842,7 +851,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>43901</v>
       </c>
@@ -858,7 +867,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43901</v>
       </c>
@@ -876,7 +885,7 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43902</v>
       </c>
@@ -894,7 +903,7 @@
       </c>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43903</v>
       </c>
@@ -914,7 +923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43905</v>
       </c>
@@ -932,7 +941,7 @@
       </c>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43906</v>
       </c>
@@ -950,15 +959,23 @@
       </c>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="5"/>
+      <c r="B20" s="1">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -966,7 +983,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -974,7 +991,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -982,7 +999,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>

</xml_diff>

<commit_message>
Création du tableaux des scores, affichage noms et scores des utilisateur et correction de bugs divers
</commit_message>
<xml_diff>
--- a/doc/journal de travail MA-20.xlsx
+++ b/doc/journal de travail MA-20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marina\Documents\CPNV\MA-20\Bataille-Navale\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPNV\MA-20\Bataille-Navale\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B854AD58-BBBA-453D-ACEE-CBAD09464BF0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42539482-AC0C-4F8E-B761-8B4538398ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4068" yWindow="132" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>J'ai visualisé des vidéos pour comment faire des fichiers et comment y écrire à l'intérieur, et le programme demande si l'utilisateur veut entrer un nom ou pas et l'affiche pendant le jeu et la fin du jeu dans le message de victoire</t>
+  </si>
+  <si>
+    <t>Un problème de switch a été trouvé. Le bug consistait que si on choisis de quitter la partie quand on a gagné, le programme va rediriger sur la partie déjà existante mais qui est déjà finie. J'ai résolu le problème en remplaçant le switch par des if avec des break à l'intérieur</t>
+  </si>
+  <si>
+    <t>Création du tableaux des scores, création du fichier contenant les noms d'utilisateurs ainsi que leurs scores et correction de bugs divers.</t>
+  </si>
+  <si>
+    <t>3h10</t>
+  </si>
+  <si>
+    <t>Explication d'une découverte de bug juste à droite ainsi qu'un autre que lorsque on retire sur un bateau une fois ses points de vie descendent meme si la case a déjà été touchée. Le bug a été corrigé. J'ai aussi regardé une suite de vidéos explicant les diverses fonctions concernant la création de fichiers.</t>
   </si>
 </sst>
 </file>
@@ -598,23 +610,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="94" zoomScaleNormal="112" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="46.88671875" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -634,7 +646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>43887</v>
       </c>
@@ -655,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>43887</v>
       </c>
@@ -673,7 +685,7 @@
       </c>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43888</v>
       </c>
@@ -691,7 +703,7 @@
       </c>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43888</v>
       </c>
@@ -709,7 +721,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43889</v>
       </c>
@@ -727,7 +739,7 @@
       </c>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43894</v>
       </c>
@@ -745,7 +757,7 @@
       </c>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43894</v>
       </c>
@@ -763,7 +775,7 @@
       </c>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>43894</v>
       </c>
@@ -781,7 +793,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>43895</v>
       </c>
@@ -799,7 +811,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>43896</v>
       </c>
@@ -817,7 +829,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>43901</v>
       </c>
@@ -835,7 +847,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43901</v>
       </c>
@@ -851,7 +863,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>43901</v>
       </c>
@@ -867,7 +879,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43901</v>
       </c>
@@ -885,7 +897,7 @@
       </c>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43902</v>
       </c>
@@ -903,7 +915,7 @@
       </c>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43903</v>
       </c>
@@ -923,7 +935,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43905</v>
       </c>
@@ -941,7 +953,7 @@
       </c>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43906</v>
       </c>
@@ -959,8 +971,10 @@
       </c>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>43908</v>
+      </c>
       <c r="B20" s="1">
         <v>6</v>
       </c>
@@ -975,15 +989,27 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>43912</v>
+      </c>
+      <c r="B21" s="1">
+        <v>6</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -991,7 +1017,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -999,7 +1025,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>

</xml_diff>

<commit_message>
recherche pour comment afficher du meilleur score jusqu'au pire
</commit_message>
<xml_diff>
--- a/doc/journal de travail MA-20.xlsx
+++ b/doc/journal de travail MA-20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPNV\MA-20\Bataille-Navale\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42539482-AC0C-4F8E-B761-8B4538398ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6919EFD-E8C7-4391-BEB4-AE8BEA668F14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4068" yWindow="132" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4068" yWindow="132" windowWidth="18264" windowHeight="11712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>Explication d'une découverte de bug juste à droite ainsi qu'un autre que lorsque on retire sur un bateau une fois ses points de vie descendent meme si la case a déjà été touchée. Le bug a été corrigé. J'ai aussi regardé une suite de vidéos explicant les diverses fonctions concernant la création de fichiers.</t>
+  </si>
+  <si>
+    <t>Recherche de solutions pour comment mettre en ordre par le meilleur score au pire dans le tableau des scores</t>
+  </si>
+  <si>
+    <t>toujours entrain d'essayer d'en trouver une</t>
   </si>
 </sst>
 </file>
@@ -610,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="94" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="C20" zoomScale="94" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,13 +1015,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="B22" s="1">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>

</xml_diff>